<commit_message>
Fixed bugs, Updated Sprint Log, Updated Report, Added Tests for User Editing
</commit_message>
<xml_diff>
--- a/Logs/Sprint Log.xlsx
+++ b/Logs/Sprint Log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20356"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\Y2\S2\Software Engineering\Assignment 1\Code\Interactive-Timetable-Map\Logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\genti\Desktop\New folder\Interactive-Timetable-Map\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC445CD-F1C1-4631-B986-B7FE3030CF7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A264A9-EDAB-43A3-9419-D3C7ED8FD1D5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F0D1336B-B5F4-478B-B08D-855F913F4C9D}"/>
   </bookViews>
@@ -20,12 +20,18 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="84">
   <si>
     <t>Estimation Points</t>
   </si>
@@ -271,6 +277,12 @@
   </si>
   <si>
     <t>Admin must be able to edit extisting user/timetable database and add new users</t>
+  </si>
+  <si>
+    <t>Fix Incompatible Code In Admin Functionality - Technical</t>
+  </si>
+  <si>
+    <t>Admin must have all necessary functionalities required</t>
   </si>
 </sst>
 </file>
@@ -371,7 +383,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -476,6 +488,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -486,7 +518,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
@@ -537,6 +569,13 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -721,7 +760,7 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3643,10 +3682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C81680F1-7DB1-4575-AE06-F3221AF87DD8}">
-  <dimension ref="A1:Q43"/>
+  <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4337,8 +4376,8 @@
         <v>43893</v>
       </c>
       <c r="G31" s="13">
-        <f>SUM(E31:E43)</f>
-        <v>12</v>
+        <f>SUM(E31:E44)</f>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -4480,36 +4519,40 @@
       <c r="D38" s="19">
         <v>2</v>
       </c>
-      <c r="E38" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="F38" s="19"/>
+      <c r="E38" s="19">
+        <v>2</v>
+      </c>
+      <c r="F38" s="20">
+        <v>43903</v>
+      </c>
       <c r="G38" s="17"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D39" s="23">
-        <v>1</v>
-      </c>
-      <c r="E39" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="F39" s="24"/>
+      <c r="A39" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="34">
+        <v>3</v>
+      </c>
+      <c r="E39" s="34">
+        <v>3</v>
+      </c>
+      <c r="F39" s="36">
+        <v>43903</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C40" s="22" t="s">
         <v>16</v>
@@ -4525,16 +4568,16 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C41" s="22" t="s">
         <v>16</v>
       </c>
       <c r="D41" s="23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E41" s="23" t="s">
         <v>1</v>
@@ -4543,16 +4586,16 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C42" s="22" t="s">
         <v>16</v>
       </c>
       <c r="D42" s="23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E42" s="23" t="s">
         <v>1</v>
@@ -4560,22 +4603,40 @@
       <c r="F42" s="24"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="31" t="s">
+      <c r="A43" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" s="23">
+        <v>1</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F43" s="24"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="31" t="s">
+      <c r="B44" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="C43" s="31" t="s">
+      <c r="C44" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="D43" s="26">
+      <c r="D44" s="26">
         <v>2</v>
       </c>
-      <c r="E43" s="26" t="s">
+      <c r="E44" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="F43" s="27"/>
+      <c r="F44" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>